<commit_message>
Atualização dos casos de uso e planeamento e testes
- Atualização dos casos de uso e planeamento e testes
</commit_message>
<xml_diff>
--- a/docs/planeamento.xlsx
+++ b/docs/planeamento.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\ptdw-gr2-2018\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E37CE708-692B-4A8A-AFF4-BCE8F03FE50A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED5FF2D-E4B8-421C-8510-6651356BAE24}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planeamento" sheetId="1" r:id="rId1"/>
@@ -94,9 +94,6 @@
   </si>
   <si>
     <t>Html</t>
-  </si>
-  <si>
-    <t>Responsabilidade (%)</t>
   </si>
   <si>
     <t>Desenvolvimento de Mockups</t>
@@ -193,6 +190,9 @@
   </si>
   <si>
     <t>6.4</t>
+  </si>
+  <si>
+    <t>Responsabilidade(%)</t>
   </si>
 </sst>
 </file>
@@ -872,17 +872,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:EU43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="U14" sqref="U14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="4.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="73.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="11.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="6.28515625" customWidth="1"/>
+    <col min="3" max="3" width="63.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.7109375" customWidth="1"/>
     <col min="13" max="121" width="2.7109375" customWidth="1"/>
     <col min="122" max="151" width="9.140625" customWidth="1"/>
   </cols>
@@ -1737,7 +1738,7 @@
         <v>4</v>
       </c>
       <c r="G4" s="46" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="H4" s="46"/>
       <c r="I4" s="46"/>
@@ -1887,7 +1888,7 @@
     <row r="5" spans="2:151" x14ac:dyDescent="0.25">
       <c r="B5" s="37"/>
       <c r="C5" s="39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5" s="22"/>
       <c r="E5" s="30"/>
@@ -2043,7 +2044,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D6" s="22">
         <v>3</v>
@@ -2068,7 +2069,7 @@
         <v>20</v>
       </c>
       <c r="K6" s="20">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="L6" s="4"/>
       <c r="M6" s="12"/>
@@ -2216,7 +2217,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D7" s="22">
         <v>0</v>
@@ -2562,7 +2563,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D9" s="22">
         <v>7</v>
@@ -2735,7 +2736,7 @@
         <v>5</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D10" s="22">
         <v>7</v>
@@ -3061,10 +3062,10 @@
     </row>
     <row r="12" spans="2:151" x14ac:dyDescent="0.25">
       <c r="B12" s="37" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C12" s="32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D12" s="22">
         <v>7</v>
@@ -3234,10 +3235,10 @@
     </row>
     <row r="13" spans="2:151" x14ac:dyDescent="0.25">
       <c r="B13" s="37" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C13" s="32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D13" s="22">
         <v>3</v>
@@ -3250,19 +3251,19 @@
         <v>43390</v>
       </c>
       <c r="G13" s="20">
+        <v>50</v>
+      </c>
+      <c r="H13" s="21">
         <v>0</v>
       </c>
-      <c r="H13" s="21">
-        <v>33</v>
-      </c>
       <c r="I13" s="21">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="J13" s="21">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="K13" s="21">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="L13" s="4"/>
       <c r="M13" s="12"/>
@@ -3407,10 +3408,10 @@
     </row>
     <row r="14" spans="2:151" x14ac:dyDescent="0.25">
       <c r="B14" s="37" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" s="32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D14" s="22">
         <v>3</v>
@@ -3422,11 +3423,21 @@
         <f t="shared" si="100"/>
         <v>43394</v>
       </c>
-      <c r="G14" s="20"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="21"/>
+      <c r="G14" s="20">
+        <v>0</v>
+      </c>
+      <c r="H14" s="21">
+        <v>33</v>
+      </c>
+      <c r="I14" s="21">
+        <v>33</v>
+      </c>
+      <c r="J14" s="21">
+        <v>33</v>
+      </c>
+      <c r="K14" s="21">
+        <v>0</v>
+      </c>
       <c r="L14" s="4"/>
       <c r="M14" s="12"/>
       <c r="N14" s="4"/>
@@ -3570,10 +3581,10 @@
     </row>
     <row r="15" spans="2:151" x14ac:dyDescent="0.25">
       <c r="B15" s="37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C15" s="32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D15" s="33">
         <v>3</v>
@@ -3586,19 +3597,19 @@
         <v>43394</v>
       </c>
       <c r="G15" s="20">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="H15" s="20">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="I15" s="20">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="J15" s="20">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K15" s="20">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="L15" s="4"/>
       <c r="M15" s="12"/>
@@ -3746,7 +3757,7 @@
         <v>7</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D16" s="33">
         <v>1</v>
@@ -4088,7 +4099,7 @@
     <row r="18" spans="2:151" x14ac:dyDescent="0.25">
       <c r="B18" s="39"/>
       <c r="C18" s="39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D18" s="22"/>
       <c r="E18" s="30"/>
@@ -4397,10 +4408,10 @@
     </row>
     <row r="20" spans="2:151" x14ac:dyDescent="0.25">
       <c r="B20" s="38" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C20" s="34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D20" s="22">
         <v>7</v>
@@ -4570,10 +4581,10 @@
     </row>
     <row r="21" spans="2:151" x14ac:dyDescent="0.25">
       <c r="B21" s="38" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C21" s="34" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D21" s="22">
         <v>14</v>
@@ -4899,7 +4910,7 @@
     </row>
     <row r="23" spans="2:151" x14ac:dyDescent="0.25">
       <c r="B23" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C23" s="32" t="s">
         <v>20</v>
@@ -5072,10 +5083,10 @@
     </row>
     <row r="24" spans="2:151" x14ac:dyDescent="0.25">
       <c r="B24" s="37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C24" s="32" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D24" s="22">
         <v>30</v>
@@ -5245,10 +5256,10 @@
     </row>
     <row r="25" spans="2:151" x14ac:dyDescent="0.25">
       <c r="B25" s="37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C25" s="32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D25" s="22">
         <v>30</v>
@@ -5418,10 +5429,10 @@
     </row>
     <row r="26" spans="2:151" x14ac:dyDescent="0.25">
       <c r="B26" s="37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C26" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D26" s="22">
         <v>30</v>
@@ -5926,7 +5937,7 @@
     <row r="29" spans="2:151" x14ac:dyDescent="0.25">
       <c r="B29" s="39"/>
       <c r="C29" s="39" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D29" s="22"/>
       <c r="E29" s="30"/>
@@ -6599,7 +6610,7 @@
     <row r="33" spans="2:151" x14ac:dyDescent="0.25">
       <c r="B33" s="39"/>
       <c r="C33" s="39" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D33" s="22">
         <v>0</v>
@@ -6772,16 +6783,16 @@
         <v>13</v>
       </c>
       <c r="H34" s="36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I34" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="J34" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="J34" s="36" t="s">
-        <v>31</v>
-      </c>
       <c r="K34" s="36" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="35" spans="2:151" x14ac:dyDescent="0.25">
@@ -6972,25 +6983,41 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EC2BBF5-5005-4D09-A03F-383FBB658F49}">
-  <dimension ref="B1:AK40"/>
+  <dimension ref="A1:Z34"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="4.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="73.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="9" width="6.28515625" customWidth="1"/>
-    <col min="10" max="37" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="26" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D1"/>
-    </row>
-    <row r="2" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15"/>
+      <c r="B2" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="46" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
       <c r="J2" s="15"/>
       <c r="K2" s="15"/>
       <c r="L2" s="15"/>
@@ -7008,19 +7035,19 @@
       <c r="X2" s="15"/>
       <c r="Y2" s="15"/>
       <c r="Z2" s="15"/>
-      <c r="AA2" s="15"/>
-      <c r="AB2" s="15"/>
-      <c r="AC2" s="15"/>
-      <c r="AD2" s="15"/>
-      <c r="AE2" s="15"/>
-      <c r="AF2" s="15"/>
-      <c r="AG2" s="15"/>
-      <c r="AH2" s="15"/>
-      <c r="AI2" s="15"/>
-      <c r="AJ2" s="15"/>
-      <c r="AK2" s="15"/>
     </row>
-    <row r="3" spans="2:37" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="40"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="22"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
       <c r="J3" s="40"/>
       <c r="K3" s="40"/>
       <c r="L3" s="40"/>
@@ -7038,35 +7065,33 @@
       <c r="X3" s="40"/>
       <c r="Y3" s="40"/>
       <c r="Z3" s="40"/>
-      <c r="AA3" s="40"/>
-      <c r="AB3" s="40"/>
-      <c r="AC3" s="40"/>
-      <c r="AD3" s="40"/>
-      <c r="AE3" s="40"/>
-      <c r="AF3" s="40"/>
-      <c r="AG3" s="40"/>
-      <c r="AH3" s="40"/>
-      <c r="AI3" s="40"/>
-      <c r="AJ3" s="40"/>
-      <c r="AK3" s="40"/>
     </row>
-    <row r="4" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B4" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="17" t="s">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A4" s="40"/>
+      <c r="B4" s="37">
         <v>1</v>
       </c>
-      <c r="D4" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="46" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
+      <c r="C4" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="22">
+        <v>3</v>
+      </c>
+      <c r="E4" s="20">
+        <v>20</v>
+      </c>
+      <c r="F4" s="20">
+        <v>20</v>
+      </c>
+      <c r="G4" s="20">
+        <v>20</v>
+      </c>
+      <c r="H4" s="20">
+        <v>20</v>
+      </c>
+      <c r="I4" s="20">
+        <v>20</v>
+      </c>
       <c r="J4" s="40"/>
       <c r="K4" s="40"/>
       <c r="L4" s="40"/>
@@ -7084,29 +7109,33 @@
       <c r="X4" s="40"/>
       <c r="Y4" s="40"/>
       <c r="Z4" s="40"/>
-      <c r="AA4" s="40"/>
-      <c r="AB4" s="40"/>
-      <c r="AC4" s="40"/>
-      <c r="AD4" s="40"/>
-      <c r="AE4" s="40"/>
-      <c r="AF4" s="40"/>
-      <c r="AG4" s="40"/>
-      <c r="AH4" s="40"/>
-      <c r="AI4" s="40"/>
-      <c r="AJ4" s="40"/>
-      <c r="AK4" s="40"/>
     </row>
-    <row r="5" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B5" s="37"/>
-      <c r="C5" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
+      <c r="B5" s="37">
+        <v>2</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="22">
+        <v>0</v>
+      </c>
+      <c r="E5" s="20">
+        <v>0</v>
+      </c>
+      <c r="F5" s="20">
+        <v>0</v>
+      </c>
+      <c r="G5" s="20">
+        <v>50</v>
+      </c>
+      <c r="H5" s="20">
+        <v>0</v>
+      </c>
+      <c r="I5" s="20">
+        <v>50</v>
+      </c>
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
       <c r="L5" s="9"/>
@@ -7124,39 +7153,29 @@
       <c r="X5" s="9"/>
       <c r="Y5" s="9"/>
       <c r="Z5" s="9"/>
-      <c r="AA5" s="9"/>
-      <c r="AB5" s="9"/>
-      <c r="AC5" s="9"/>
-      <c r="AD5" s="9"/>
-      <c r="AE5" s="9"/>
-      <c r="AF5" s="9"/>
-      <c r="AG5" s="9"/>
-      <c r="AH5" s="9"/>
-      <c r="AI5" s="9"/>
-      <c r="AJ5" s="9"/>
-      <c r="AK5" s="9"/>
     </row>
-    <row r="6" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A6" s="9"/>
       <c r="B6" s="37">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="D6" s="22">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E6" s="20">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F6" s="20">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="G6" s="20">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="H6" s="20">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="I6" s="20">
         <v>0</v>
@@ -7178,36 +7197,26 @@
       <c r="X6" s="9"/>
       <c r="Y6" s="9"/>
       <c r="Z6" s="9"/>
-      <c r="AA6" s="9"/>
-      <c r="AB6" s="9"/>
-      <c r="AC6" s="9"/>
-      <c r="AD6" s="9"/>
-      <c r="AE6" s="9"/>
-      <c r="AF6" s="9"/>
-      <c r="AG6" s="9"/>
-      <c r="AH6" s="9"/>
-      <c r="AI6" s="9"/>
-      <c r="AJ6" s="9"/>
-      <c r="AK6" s="9"/>
     </row>
-    <row r="7" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
       <c r="B7" s="37">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C7" s="29" t="s">
         <v>46</v>
       </c>
       <c r="D7" s="22">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E7" s="20">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F7" s="20">
         <v>0</v>
       </c>
       <c r="G7" s="20">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="H7" s="20">
         <v>0</v>
@@ -7232,42 +7241,32 @@
       <c r="X7" s="9"/>
       <c r="Y7" s="9"/>
       <c r="Z7" s="9"/>
-      <c r="AA7" s="9"/>
-      <c r="AB7" s="9"/>
-      <c r="AC7" s="9"/>
-      <c r="AD7" s="9"/>
-      <c r="AE7" s="9"/>
-      <c r="AF7" s="9"/>
-      <c r="AG7" s="9"/>
-      <c r="AH7" s="9"/>
-      <c r="AI7" s="9"/>
-      <c r="AJ7" s="9"/>
-      <c r="AK7" s="9"/>
     </row>
-    <row r="8" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
       <c r="B8" s="37">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="D8" s="22">
         <v>7</v>
       </c>
       <c r="E8" s="20">
+        <v>50</v>
+      </c>
+      <c r="F8" s="21">
         <v>0</v>
       </c>
-      <c r="F8" s="20">
-        <v>33</v>
-      </c>
-      <c r="G8" s="20">
-        <v>33</v>
-      </c>
-      <c r="H8" s="20">
-        <v>33</v>
-      </c>
-      <c r="I8" s="20">
+      <c r="G8" s="21">
         <v>0</v>
+      </c>
+      <c r="H8" s="21">
+        <v>0</v>
+      </c>
+      <c r="I8" s="21">
+        <v>50</v>
       </c>
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
@@ -7286,43 +7285,21 @@
       <c r="X8" s="9"/>
       <c r="Y8" s="9"/>
       <c r="Z8" s="9"/>
-      <c r="AA8" s="9"/>
-      <c r="AB8" s="9"/>
-      <c r="AC8" s="9"/>
-      <c r="AD8" s="9"/>
-      <c r="AE8" s="9"/>
-      <c r="AF8" s="9"/>
-      <c r="AG8" s="9"/>
-      <c r="AH8" s="9"/>
-      <c r="AI8" s="9"/>
-      <c r="AJ8" s="9"/>
-      <c r="AK8" s="9"/>
     </row>
-    <row r="9" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B9" s="37">
-        <v>4</v>
-      </c>
-      <c r="C9" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="D9" s="22">
-        <v>7</v>
-      </c>
-      <c r="E9" s="20">
-        <v>50</v>
-      </c>
-      <c r="F9" s="20">
-        <v>0</v>
-      </c>
-      <c r="G9" s="20">
-        <v>0</v>
-      </c>
-      <c r="H9" s="20">
-        <v>0</v>
-      </c>
-      <c r="I9" s="20">
-        <v>50</v>
-      </c>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9" s="9"/>
+      <c r="B9" s="38">
+        <v>6</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="22"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
       <c r="L9" s="9"/>
@@ -7340,42 +7317,32 @@
       <c r="X9" s="9"/>
       <c r="Y9" s="9"/>
       <c r="Z9" s="9"/>
-      <c r="AA9" s="9"/>
-      <c r="AB9" s="9"/>
-      <c r="AC9" s="9"/>
-      <c r="AD9" s="9"/>
-      <c r="AE9" s="9"/>
-      <c r="AF9" s="9"/>
-      <c r="AG9" s="9"/>
-      <c r="AH9" s="9"/>
-      <c r="AI9" s="9"/>
-      <c r="AJ9" s="9"/>
-      <c r="AK9" s="9"/>
     </row>
-    <row r="10" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B10" s="37">
-        <v>5</v>
-      </c>
-      <c r="C10" s="29" t="s">
-        <v>41</v>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A10" s="9"/>
+      <c r="B10" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>21</v>
       </c>
       <c r="D10" s="22">
         <v>7</v>
       </c>
       <c r="E10" s="20">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="F10" s="21">
+        <v>33</v>
+      </c>
+      <c r="G10" s="21">
+        <v>33</v>
+      </c>
+      <c r="H10" s="21">
+        <v>33</v>
+      </c>
+      <c r="I10" s="21">
         <v>0</v>
-      </c>
-      <c r="G10" s="21">
-        <v>0</v>
-      </c>
-      <c r="H10" s="21">
-        <v>0</v>
-      </c>
-      <c r="I10" s="21">
-        <v>50</v>
       </c>
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
@@ -7394,31 +7361,33 @@
       <c r="X10" s="9"/>
       <c r="Y10" s="9"/>
       <c r="Z10" s="9"/>
-      <c r="AA10" s="9"/>
-      <c r="AB10" s="9"/>
-      <c r="AC10" s="9"/>
-      <c r="AD10" s="9"/>
-      <c r="AE10" s="9"/>
-      <c r="AF10" s="9"/>
-      <c r="AG10" s="9"/>
-      <c r="AH10" s="9"/>
-      <c r="AI10" s="9"/>
-      <c r="AJ10" s="9"/>
-      <c r="AK10" s="9"/>
     </row>
-    <row r="11" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B11" s="38">
-        <v>6</v>
-      </c>
-      <c r="C11" s="31" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="22"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="21"/>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
+      <c r="B11" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="22">
+        <v>3</v>
+      </c>
+      <c r="E11" s="20">
+        <v>50</v>
+      </c>
+      <c r="F11" s="21">
+        <v>0</v>
+      </c>
+      <c r="G11" s="21">
+        <v>0</v>
+      </c>
+      <c r="H11" s="21">
+        <v>0</v>
+      </c>
+      <c r="I11" s="21">
+        <v>50</v>
+      </c>
       <c r="J11" s="9"/>
       <c r="K11" s="9"/>
       <c r="L11" s="9"/>
@@ -7436,27 +7405,17 @@
       <c r="X11" s="9"/>
       <c r="Y11" s="9"/>
       <c r="Z11" s="9"/>
-      <c r="AA11" s="9"/>
-      <c r="AB11" s="9"/>
-      <c r="AC11" s="9"/>
-      <c r="AD11" s="9"/>
-      <c r="AE11" s="9"/>
-      <c r="AF11" s="9"/>
-      <c r="AG11" s="9"/>
-      <c r="AH11" s="9"/>
-      <c r="AI11" s="9"/>
-      <c r="AJ11" s="9"/>
-      <c r="AK11" s="9"/>
     </row>
-    <row r="12" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
       <c r="B12" s="37" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C12" s="32" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="D12" s="22">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E12" s="20">
         <v>0</v>
@@ -7490,42 +7449,32 @@
       <c r="X12" s="9"/>
       <c r="Y12" s="9"/>
       <c r="Z12" s="9"/>
-      <c r="AA12" s="9"/>
-      <c r="AB12" s="9"/>
-      <c r="AC12" s="9"/>
-      <c r="AD12" s="9"/>
-      <c r="AE12" s="9"/>
-      <c r="AF12" s="9"/>
-      <c r="AG12" s="9"/>
-      <c r="AH12" s="9"/>
-      <c r="AI12" s="9"/>
-      <c r="AJ12" s="9"/>
-      <c r="AK12" s="9"/>
     </row>
-    <row r="13" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A13" s="9"/>
       <c r="B13" s="37" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C13" s="32" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="22">
+        <v>48</v>
+      </c>
+      <c r="D13" s="33">
         <v>3</v>
       </c>
       <c r="E13" s="20">
+        <v>50</v>
+      </c>
+      <c r="F13" s="20">
         <v>0</v>
       </c>
-      <c r="F13" s="21">
-        <v>33</v>
-      </c>
-      <c r="G13" s="21">
-        <v>33</v>
-      </c>
-      <c r="H13" s="21">
-        <v>33</v>
-      </c>
-      <c r="I13" s="21">
+      <c r="G13" s="20">
         <v>0</v>
+      </c>
+      <c r="H13" s="20">
+        <v>0</v>
+      </c>
+      <c r="I13" s="20">
+        <v>50</v>
       </c>
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
@@ -7544,33 +7493,33 @@
       <c r="X13" s="9"/>
       <c r="Y13" s="9"/>
       <c r="Z13" s="9"/>
-      <c r="AA13" s="9"/>
-      <c r="AB13" s="9"/>
-      <c r="AC13" s="9"/>
-      <c r="AD13" s="9"/>
-      <c r="AE13" s="9"/>
-      <c r="AF13" s="9"/>
-      <c r="AG13" s="9"/>
-      <c r="AH13" s="9"/>
-      <c r="AI13" s="9"/>
-      <c r="AJ13" s="9"/>
-      <c r="AK13" s="9"/>
     </row>
-    <row r="14" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B14" s="37" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="D14" s="22">
-        <v>3</v>
-      </c>
-      <c r="E14" s="20"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="21"/>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A14" s="9"/>
+      <c r="B14" s="37">
+        <v>7</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="33">
+        <v>1</v>
+      </c>
+      <c r="E14" s="20">
+        <v>20</v>
+      </c>
+      <c r="F14" s="20">
+        <v>20</v>
+      </c>
+      <c r="G14" s="20">
+        <v>20</v>
+      </c>
+      <c r="H14" s="20">
+        <v>20</v>
+      </c>
+      <c r="I14" s="20">
+        <v>20</v>
+      </c>
       <c r="J14" s="9"/>
       <c r="K14" s="9"/>
       <c r="L14" s="9"/>
@@ -7588,27 +7537,15 @@
       <c r="X14" s="9"/>
       <c r="Y14" s="9"/>
       <c r="Z14" s="9"/>
-      <c r="AA14" s="9"/>
-      <c r="AB14" s="9"/>
-      <c r="AC14" s="9"/>
-      <c r="AD14" s="9"/>
-      <c r="AE14" s="9"/>
-      <c r="AF14" s="9"/>
-      <c r="AG14" s="9"/>
-      <c r="AH14" s="9"/>
-      <c r="AI14" s="9"/>
-      <c r="AJ14" s="9"/>
-      <c r="AK14" s="9"/>
     </row>
-    <row r="15" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B15" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" s="32" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15" s="33">
-        <v>3</v>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A15" s="9"/>
+      <c r="B15" s="39"/>
+      <c r="C15" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="22">
+        <v>0</v>
       </c>
       <c r="E15" s="20">
         <v>20</v>
@@ -7642,43 +7579,19 @@
       <c r="X15" s="9"/>
       <c r="Y15" s="9"/>
       <c r="Z15" s="9"/>
-      <c r="AA15" s="9"/>
-      <c r="AB15" s="9"/>
-      <c r="AC15" s="9"/>
-      <c r="AD15" s="9"/>
-      <c r="AE15" s="9"/>
-      <c r="AF15" s="9"/>
-      <c r="AG15" s="9"/>
-      <c r="AH15" s="9"/>
-      <c r="AI15" s="9"/>
-      <c r="AJ15" s="9"/>
-      <c r="AK15" s="9"/>
     </row>
-    <row r="16" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B16" s="37">
-        <v>7</v>
-      </c>
-      <c r="C16" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="33">
-        <v>1</v>
-      </c>
-      <c r="E16" s="20">
-        <v>20</v>
-      </c>
-      <c r="F16" s="20">
-        <v>20</v>
-      </c>
-      <c r="G16" s="20">
-        <v>20</v>
-      </c>
-      <c r="H16" s="20">
-        <v>20</v>
-      </c>
-      <c r="I16" s="20">
-        <v>20</v>
-      </c>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A16" s="9"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="22"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
       <c r="L16" s="9"/>
@@ -7696,41 +7609,21 @@
       <c r="X16" s="9"/>
       <c r="Y16" s="9"/>
       <c r="Z16" s="9"/>
-      <c r="AA16" s="9"/>
-      <c r="AB16" s="9"/>
-      <c r="AC16" s="9"/>
-      <c r="AD16" s="9"/>
-      <c r="AE16" s="9"/>
-      <c r="AF16" s="9"/>
-      <c r="AG16" s="9"/>
-      <c r="AH16" s="9"/>
-      <c r="AI16" s="9"/>
-      <c r="AJ16" s="9"/>
-      <c r="AK16" s="9"/>
     </row>
-    <row r="17" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B17" s="39"/>
-      <c r="C17" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="22">
-        <v>0</v>
-      </c>
-      <c r="E17" s="20">
-        <v>20</v>
-      </c>
-      <c r="F17" s="20">
-        <v>20</v>
-      </c>
-      <c r="G17" s="20">
-        <v>20</v>
-      </c>
-      <c r="H17" s="20">
-        <v>20</v>
-      </c>
-      <c r="I17" s="20">
-        <v>20</v>
-      </c>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A17" s="9"/>
+      <c r="B17" s="38">
+        <v>8</v>
+      </c>
+      <c r="C17" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="22"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
       <c r="J17" s="9"/>
       <c r="K17" s="9"/>
       <c r="L17" s="9"/>
@@ -7748,29 +7641,33 @@
       <c r="X17" s="9"/>
       <c r="Y17" s="9"/>
       <c r="Z17" s="9"/>
-      <c r="AA17" s="9"/>
-      <c r="AB17" s="9"/>
-      <c r="AC17" s="9"/>
-      <c r="AD17" s="9"/>
-      <c r="AE17" s="9"/>
-      <c r="AF17" s="9"/>
-      <c r="AG17" s="9"/>
-      <c r="AH17" s="9"/>
-      <c r="AI17" s="9"/>
-      <c r="AJ17" s="9"/>
-      <c r="AK17" s="9"/>
     </row>
-    <row r="18" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B18" s="39"/>
-      <c r="C18" s="39" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" s="22"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A18" s="9"/>
+      <c r="B18" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="22">
+        <v>7</v>
+      </c>
+      <c r="E18" s="21">
+        <v>50</v>
+      </c>
+      <c r="F18" s="20">
+        <v>0</v>
+      </c>
+      <c r="G18" s="21">
+        <v>0</v>
+      </c>
+      <c r="H18" s="20">
+        <v>0</v>
+      </c>
+      <c r="I18" s="20">
+        <v>50</v>
+      </c>
       <c r="J18" s="9"/>
       <c r="K18" s="9"/>
       <c r="L18" s="9"/>
@@ -7788,31 +7685,33 @@
       <c r="X18" s="9"/>
       <c r="Y18" s="9"/>
       <c r="Z18" s="9"/>
-      <c r="AA18" s="9"/>
-      <c r="AB18" s="9"/>
-      <c r="AC18" s="9"/>
-      <c r="AD18" s="9"/>
-      <c r="AE18" s="9"/>
-      <c r="AF18" s="9"/>
-      <c r="AG18" s="9"/>
-      <c r="AH18" s="9"/>
-      <c r="AI18" s="9"/>
-      <c r="AJ18" s="9"/>
-      <c r="AK18" s="9"/>
     </row>
-    <row r="19" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B19" s="38">
-        <v>8</v>
-      </c>
-      <c r="C19" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="22"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A19" s="9"/>
+      <c r="B19" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="22">
+        <v>14</v>
+      </c>
+      <c r="E19" s="21">
+        <v>50</v>
+      </c>
+      <c r="F19" s="20">
+        <v>0</v>
+      </c>
+      <c r="G19" s="21">
+        <v>0</v>
+      </c>
+      <c r="H19" s="20">
+        <v>0</v>
+      </c>
+      <c r="I19" s="20">
+        <v>50</v>
+      </c>
       <c r="J19" s="9"/>
       <c r="K19" s="9"/>
       <c r="L19" s="9"/>
@@ -7830,43 +7729,21 @@
       <c r="X19" s="9"/>
       <c r="Y19" s="9"/>
       <c r="Z19" s="9"/>
-      <c r="AA19" s="9"/>
-      <c r="AB19" s="9"/>
-      <c r="AC19" s="9"/>
-      <c r="AD19" s="9"/>
-      <c r="AE19" s="9"/>
-      <c r="AF19" s="9"/>
-      <c r="AG19" s="9"/>
-      <c r="AH19" s="9"/>
-      <c r="AI19" s="9"/>
-      <c r="AJ19" s="9"/>
-      <c r="AK19" s="9"/>
     </row>
-    <row r="20" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B20" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20" s="22">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A20" s="9"/>
+      <c r="B20" s="38">
+        <v>9</v>
+      </c>
+      <c r="C20" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="21">
-        <v>50</v>
-      </c>
-      <c r="F20" s="20">
-        <v>0</v>
-      </c>
-      <c r="G20" s="21">
-        <v>0</v>
-      </c>
-      <c r="H20" s="20">
-        <v>0</v>
-      </c>
-      <c r="I20" s="20">
-        <v>50</v>
-      </c>
+      <c r="D20" s="22"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="21"/>
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
       <c r="L20" s="9"/>
@@ -7884,42 +7761,32 @@
       <c r="X20" s="9"/>
       <c r="Y20" s="9"/>
       <c r="Z20" s="9"/>
-      <c r="AA20" s="9"/>
-      <c r="AB20" s="9"/>
-      <c r="AC20" s="9"/>
-      <c r="AD20" s="9"/>
-      <c r="AE20" s="9"/>
-      <c r="AF20" s="9"/>
-      <c r="AG20" s="9"/>
-      <c r="AH20" s="9"/>
-      <c r="AI20" s="9"/>
-      <c r="AJ20" s="9"/>
-      <c r="AK20" s="9"/>
     </row>
-    <row r="21" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B21" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" s="34" t="s">
-        <v>26</v>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A21" s="9"/>
+      <c r="B21" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="32" t="s">
+        <v>20</v>
       </c>
       <c r="D21" s="22">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="E21" s="21">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="F21" s="20">
-        <v>0</v>
-      </c>
-      <c r="G21" s="21">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="G21" s="20">
+        <v>20</v>
       </c>
       <c r="H21" s="20">
-        <v>0</v>
-      </c>
-      <c r="I21" s="20">
-        <v>50</v>
+        <v>20</v>
+      </c>
+      <c r="I21" s="21">
+        <v>20</v>
       </c>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
@@ -7938,31 +7805,33 @@
       <c r="X21" s="9"/>
       <c r="Y21" s="9"/>
       <c r="Z21" s="9"/>
-      <c r="AA21" s="9"/>
-      <c r="AB21" s="9"/>
-      <c r="AC21" s="9"/>
-      <c r="AD21" s="9"/>
-      <c r="AE21" s="9"/>
-      <c r="AF21" s="9"/>
-      <c r="AG21" s="9"/>
-      <c r="AH21" s="9"/>
-      <c r="AI21" s="9"/>
-      <c r="AJ21" s="9"/>
-      <c r="AK21" s="9"/>
     </row>
-    <row r="22" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B22" s="38">
-        <v>9</v>
-      </c>
-      <c r="C22" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" s="22"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="21"/>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A22" s="9"/>
+      <c r="B22" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="22">
+        <v>30</v>
+      </c>
+      <c r="E22" s="21">
+        <v>20</v>
+      </c>
+      <c r="F22" s="20">
+        <v>20</v>
+      </c>
+      <c r="G22" s="20">
+        <v>20</v>
+      </c>
+      <c r="H22" s="20">
+        <v>20</v>
+      </c>
+      <c r="I22" s="21">
+        <v>20</v>
+      </c>
       <c r="J22" s="9"/>
       <c r="K22" s="9"/>
       <c r="L22" s="9"/>
@@ -7980,24 +7849,14 @@
       <c r="X22" s="9"/>
       <c r="Y22" s="9"/>
       <c r="Z22" s="9"/>
-      <c r="AA22" s="9"/>
-      <c r="AB22" s="9"/>
-      <c r="AC22" s="9"/>
-      <c r="AD22" s="9"/>
-      <c r="AE22" s="9"/>
-      <c r="AF22" s="9"/>
-      <c r="AG22" s="9"/>
-      <c r="AH22" s="9"/>
-      <c r="AI22" s="9"/>
-      <c r="AJ22" s="9"/>
-      <c r="AK22" s="9"/>
     </row>
-    <row r="23" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A23" s="9"/>
       <c r="B23" s="37" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C23" s="32" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D23" s="22">
         <v>30</v>
@@ -8034,24 +7893,14 @@
       <c r="X23" s="9"/>
       <c r="Y23" s="9"/>
       <c r="Z23" s="9"/>
-      <c r="AA23" s="9"/>
-      <c r="AB23" s="9"/>
-      <c r="AC23" s="9"/>
-      <c r="AD23" s="9"/>
-      <c r="AE23" s="9"/>
-      <c r="AF23" s="9"/>
-      <c r="AG23" s="9"/>
-      <c r="AH23" s="9"/>
-      <c r="AI23" s="9"/>
-      <c r="AJ23" s="9"/>
-      <c r="AK23" s="9"/>
     </row>
-    <row r="24" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A24" s="9"/>
       <c r="B24" s="37" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C24" s="32" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D24" s="22">
         <v>30</v>
@@ -8088,29 +7937,19 @@
       <c r="X24" s="9"/>
       <c r="Y24" s="9"/>
       <c r="Z24" s="9"/>
-      <c r="AA24" s="9"/>
-      <c r="AB24" s="9"/>
-      <c r="AC24" s="9"/>
-      <c r="AD24" s="9"/>
-      <c r="AE24" s="9"/>
-      <c r="AF24" s="9"/>
-      <c r="AG24" s="9"/>
-      <c r="AH24" s="9"/>
-      <c r="AI24" s="9"/>
-      <c r="AJ24" s="9"/>
-      <c r="AK24" s="9"/>
     </row>
-    <row r="25" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B25" s="37" t="s">
-        <v>39</v>
-      </c>
-      <c r="C25" s="32" t="s">
-        <v>24</v>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A25" s="9"/>
+      <c r="B25" s="37">
+        <v>10</v>
+      </c>
+      <c r="C25" s="29" t="s">
+        <v>11</v>
       </c>
       <c r="D25" s="22">
-        <v>30</v>
-      </c>
-      <c r="E25" s="21">
+        <v>4</v>
+      </c>
+      <c r="E25" s="20">
         <v>20</v>
       </c>
       <c r="F25" s="20">
@@ -8122,7 +7961,7 @@
       <c r="H25" s="20">
         <v>20</v>
       </c>
-      <c r="I25" s="21">
+      <c r="I25" s="20">
         <v>20</v>
       </c>
       <c r="J25" s="9"/>
@@ -8142,43 +7981,21 @@
       <c r="X25" s="9"/>
       <c r="Y25" s="9"/>
       <c r="Z25" s="9"/>
-      <c r="AA25" s="9"/>
-      <c r="AB25" s="9"/>
-      <c r="AC25" s="9"/>
-      <c r="AD25" s="9"/>
-      <c r="AE25" s="9"/>
-      <c r="AF25" s="9"/>
-      <c r="AG25" s="9"/>
-      <c r="AH25" s="9"/>
-      <c r="AI25" s="9"/>
-      <c r="AJ25" s="9"/>
-      <c r="AK25" s="9"/>
     </row>
-    <row r="26" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B26" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="C26" s="32" t="s">
-        <v>27</v>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A26" s="9"/>
+      <c r="B26" s="39"/>
+      <c r="C26" s="39" t="s">
+        <v>19</v>
       </c>
       <c r="D26" s="22">
-        <v>30</v>
-      </c>
-      <c r="E26" s="21">
-        <v>20</v>
-      </c>
-      <c r="F26" s="20">
-        <v>20</v>
-      </c>
-      <c r="G26" s="20">
-        <v>20</v>
-      </c>
-      <c r="H26" s="20">
-        <v>20</v>
-      </c>
-      <c r="I26" s="21">
-        <v>20</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="21"/>
       <c r="J26" s="9"/>
       <c r="K26" s="9"/>
       <c r="L26" s="9"/>
@@ -8196,43 +8013,19 @@
       <c r="X26" s="9"/>
       <c r="Y26" s="9"/>
       <c r="Z26" s="9"/>
-      <c r="AA26" s="9"/>
-      <c r="AB26" s="9"/>
-      <c r="AC26" s="9"/>
-      <c r="AD26" s="9"/>
-      <c r="AE26" s="9"/>
-      <c r="AF26" s="9"/>
-      <c r="AG26" s="9"/>
-      <c r="AH26" s="9"/>
-      <c r="AI26" s="9"/>
-      <c r="AJ26" s="9"/>
-      <c r="AK26" s="9"/>
     </row>
-    <row r="27" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B27" s="37">
-        <v>10</v>
-      </c>
-      <c r="C27" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27" s="22">
-        <v>4</v>
-      </c>
-      <c r="E27" s="20">
-        <v>20</v>
-      </c>
-      <c r="F27" s="20">
-        <v>20</v>
-      </c>
-      <c r="G27" s="20">
-        <v>20</v>
-      </c>
-      <c r="H27" s="20">
-        <v>20</v>
-      </c>
-      <c r="I27" s="20">
-        <v>20</v>
-      </c>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A27" s="9"/>
+      <c r="B27" s="39"/>
+      <c r="C27" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" s="22"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21"/>
       <c r="J27" s="9"/>
       <c r="K27" s="9"/>
       <c r="L27" s="9"/>
@@ -8250,31 +8043,33 @@
       <c r="X27" s="9"/>
       <c r="Y27" s="9"/>
       <c r="Z27" s="9"/>
-      <c r="AA27" s="9"/>
-      <c r="AB27" s="9"/>
-      <c r="AC27" s="9"/>
-      <c r="AD27" s="9"/>
-      <c r="AE27" s="9"/>
-      <c r="AF27" s="9"/>
-      <c r="AG27" s="9"/>
-      <c r="AH27" s="9"/>
-      <c r="AI27" s="9"/>
-      <c r="AJ27" s="9"/>
-      <c r="AK27" s="9"/>
     </row>
-    <row r="28" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B28" s="39"/>
-      <c r="C28" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="D28" s="22">
-        <v>0</v>
-      </c>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="21"/>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A28" s="9"/>
+      <c r="B28" s="37">
+        <v>11</v>
+      </c>
+      <c r="C28" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="35">
+        <v>10</v>
+      </c>
+      <c r="E28" s="20">
+        <v>20</v>
+      </c>
+      <c r="F28" s="20">
+        <v>20</v>
+      </c>
+      <c r="G28" s="20">
+        <v>20</v>
+      </c>
+      <c r="H28" s="20">
+        <v>20</v>
+      </c>
+      <c r="I28" s="20">
+        <v>20</v>
+      </c>
       <c r="J28" s="9"/>
       <c r="K28" s="9"/>
       <c r="L28" s="9"/>
@@ -8292,29 +8087,33 @@
       <c r="X28" s="9"/>
       <c r="Y28" s="9"/>
       <c r="Z28" s="9"/>
-      <c r="AA28" s="9"/>
-      <c r="AB28" s="9"/>
-      <c r="AC28" s="9"/>
-      <c r="AD28" s="9"/>
-      <c r="AE28" s="9"/>
-      <c r="AF28" s="9"/>
-      <c r="AG28" s="9"/>
-      <c r="AH28" s="9"/>
-      <c r="AI28" s="9"/>
-      <c r="AJ28" s="9"/>
-      <c r="AK28" s="9"/>
     </row>
-    <row r="29" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B29" s="39"/>
-      <c r="C29" s="39" t="s">
-        <v>44</v>
-      </c>
-      <c r="D29" s="22"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="21"/>
-      <c r="I29" s="21"/>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A29" s="9"/>
+      <c r="B29" s="37">
+        <v>12</v>
+      </c>
+      <c r="C29" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="22">
+        <v>15</v>
+      </c>
+      <c r="E29" s="20">
+        <v>20</v>
+      </c>
+      <c r="F29" s="20">
+        <v>20</v>
+      </c>
+      <c r="G29" s="20">
+        <v>20</v>
+      </c>
+      <c r="H29" s="20">
+        <v>20</v>
+      </c>
+      <c r="I29" s="20">
+        <v>20</v>
+      </c>
       <c r="J29" s="9"/>
       <c r="K29" s="9"/>
       <c r="L29" s="9"/>
@@ -8332,27 +8131,17 @@
       <c r="X29" s="9"/>
       <c r="Y29" s="9"/>
       <c r="Z29" s="9"/>
-      <c r="AA29" s="9"/>
-      <c r="AB29" s="9"/>
-      <c r="AC29" s="9"/>
-      <c r="AD29" s="9"/>
-      <c r="AE29" s="9"/>
-      <c r="AF29" s="9"/>
-      <c r="AG29" s="9"/>
-      <c r="AH29" s="9"/>
-      <c r="AI29" s="9"/>
-      <c r="AJ29" s="9"/>
-      <c r="AK29" s="9"/>
     </row>
-    <row r="30" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A30" s="9"/>
       <c r="B30" s="37">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30" s="35">
         <v>10</v>
+      </c>
+      <c r="D30" s="22">
+        <v>7</v>
       </c>
       <c r="E30" s="20">
         <v>20</v>
@@ -8386,27 +8175,15 @@
       <c r="X30" s="9"/>
       <c r="Y30" s="9"/>
       <c r="Z30" s="9"/>
-      <c r="AA30" s="9"/>
-      <c r="AB30" s="9"/>
-      <c r="AC30" s="9"/>
-      <c r="AD30" s="9"/>
-      <c r="AE30" s="9"/>
-      <c r="AF30" s="9"/>
-      <c r="AG30" s="9"/>
-      <c r="AH30" s="9"/>
-      <c r="AI30" s="9"/>
-      <c r="AJ30" s="9"/>
-      <c r="AK30" s="9"/>
     </row>
-    <row r="31" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B31" s="37">
-        <v>12</v>
-      </c>
-      <c r="C31" s="29" t="s">
-        <v>9</v>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A31" s="9"/>
+      <c r="B31" s="39"/>
+      <c r="C31" s="39" t="s">
+        <v>27</v>
       </c>
       <c r="D31" s="22">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="E31" s="20">
         <v>20</v>
@@ -8440,42 +8217,26 @@
       <c r="X31" s="9"/>
       <c r="Y31" s="9"/>
       <c r="Z31" s="9"/>
-      <c r="AA31" s="9"/>
-      <c r="AB31" s="9"/>
-      <c r="AC31" s="9"/>
-      <c r="AD31" s="9"/>
-      <c r="AE31" s="9"/>
-      <c r="AF31" s="9"/>
-      <c r="AG31" s="9"/>
-      <c r="AH31" s="9"/>
-      <c r="AI31" s="9"/>
-      <c r="AJ31" s="9"/>
-      <c r="AK31" s="9"/>
     </row>
-    <row r="32" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B32" s="37">
+    <row r="32" spans="1:26" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="9"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="C32" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="D32" s="22">
-        <v>7</v>
-      </c>
-      <c r="E32" s="20">
-        <v>20</v>
-      </c>
-      <c r="F32" s="20">
-        <v>20</v>
-      </c>
-      <c r="G32" s="20">
-        <v>20</v>
-      </c>
-      <c r="H32" s="20">
-        <v>20</v>
-      </c>
-      <c r="I32" s="20">
-        <v>20</v>
+      <c r="F32" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="G32" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="H32" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="I32" s="36" t="s">
+        <v>28</v>
       </c>
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
@@ -8494,41 +8255,17 @@
       <c r="X32" s="9"/>
       <c r="Y32" s="9"/>
       <c r="Z32" s="9"/>
-      <c r="AA32" s="9"/>
-      <c r="AB32" s="9"/>
-      <c r="AC32" s="9"/>
-      <c r="AD32" s="9"/>
-      <c r="AE32" s="9"/>
-      <c r="AF32" s="9"/>
-      <c r="AG32" s="9"/>
-      <c r="AH32" s="9"/>
-      <c r="AI32" s="9"/>
-      <c r="AJ32" s="9"/>
-      <c r="AK32" s="9"/>
     </row>
-    <row r="33" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B33" s="39"/>
-      <c r="C33" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="D33" s="22">
-        <v>0</v>
-      </c>
-      <c r="E33" s="20">
-        <v>20</v>
-      </c>
-      <c r="F33" s="20">
-        <v>20</v>
-      </c>
-      <c r="G33" s="20">
-        <v>20</v>
-      </c>
-      <c r="H33" s="20">
-        <v>20</v>
-      </c>
-      <c r="I33" s="20">
-        <v>20</v>
-      </c>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A33" s="9"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
       <c r="J33" s="9"/>
       <c r="K33" s="9"/>
       <c r="L33" s="9"/>
@@ -8546,84 +8283,29 @@
       <c r="X33" s="9"/>
       <c r="Y33" s="9"/>
       <c r="Z33" s="9"/>
-      <c r="AA33" s="9"/>
-      <c r="AB33" s="9"/>
-      <c r="AC33" s="9"/>
-      <c r="AD33" s="9"/>
-      <c r="AE33" s="9"/>
-      <c r="AF33" s="9"/>
-      <c r="AG33" s="9"/>
-      <c r="AH33" s="9"/>
-      <c r="AI33" s="9"/>
-      <c r="AJ33" s="9"/>
-      <c r="AK33" s="9"/>
     </row>
-    <row r="34" spans="2:37" ht="81" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E34" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="F34" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="G34" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="H34" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="I34" s="36" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="35" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B35"/>
-    </row>
-    <row r="36" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B36" s="16"/>
-    </row>
-    <row r="37" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B37" s="4"/>
-    </row>
-    <row r="38" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B38" s="9"/>
-    </row>
-    <row r="39" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B39"/>
-    </row>
-    <row r="40" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B40"/>
-    </row>
+    <row r="34" spans="1:26" ht="81" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="29">
+  <mergeCells count="19">
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="A3:A4"/>
     <mergeCell ref="J3:J4"/>
     <mergeCell ref="K3:K4"/>
     <mergeCell ref="L3:L4"/>
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="Z3:Z4"/>
+    <mergeCell ref="T3:T4"/>
     <mergeCell ref="U3:U4"/>
     <mergeCell ref="V3:V4"/>
     <mergeCell ref="W3:W4"/>
     <mergeCell ref="X3:X4"/>
-    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="Y3:Y4"/>
     <mergeCell ref="N3:N4"/>
     <mergeCell ref="O3:O4"/>
     <mergeCell ref="P3:P4"/>
     <mergeCell ref="Q3:Q4"/>
     <mergeCell ref="R3:R4"/>
-    <mergeCell ref="AK3:AK4"/>
-    <mergeCell ref="E4:I4"/>
-    <mergeCell ref="AE3:AE4"/>
-    <mergeCell ref="AF3:AF4"/>
-    <mergeCell ref="AG3:AG4"/>
-    <mergeCell ref="AH3:AH4"/>
-    <mergeCell ref="AI3:AI4"/>
-    <mergeCell ref="AJ3:AJ4"/>
-    <mergeCell ref="Y3:Y4"/>
-    <mergeCell ref="Z3:Z4"/>
-    <mergeCell ref="AA3:AA4"/>
-    <mergeCell ref="AB3:AB4"/>
-    <mergeCell ref="AC3:AC4"/>
-    <mergeCell ref="AD3:AD4"/>
     <mergeCell ref="S3:S4"/>
-    <mergeCell ref="T3:T4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>